<commit_message>
Fix de la commande correction entièrement, amélioration du reactionlistener et optimisations en tous genre
</commit_message>
<xml_diff>
--- a/Config/Hmw_Tables/math.xlsx
+++ b/Config/Hmw_Tables/math.xlsx
@@ -14,39 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Activité 112</t>
   </si>
   <si>
+    <t>Activité 23</t>
+  </si>
+  <si>
+    <t>Activité 111</t>
+  </si>
+  <si>
     <t>Activité 11</t>
   </si>
   <si>
-    <t>Activité 111</t>
-  </si>
-  <si>
-    <t>Activité 23</t>
-  </si>
-  <si>
     <t>Élèves</t>
   </si>
   <si>
     <t>Sloth</t>
   </si>
   <si>
-    <t>le 17/05 à 16:55</t>
-  </si>
-  <si>
-    <t>Reçu</t>
+    <t>le 21/05 à 17:24</t>
+  </si>
+  <si>
+    <t>le 21/05 à 17:25</t>
   </si>
   <si>
     <t>Corrigé</t>
   </si>
   <si>
+    <t>Non rendu</t>
+  </si>
+  <si>
     <t>Skido</t>
-  </si>
-  <si>
-    <t>Non rendu</t>
   </si>
 </sst>
 </file>
@@ -70,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,12 +98,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFDFB3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBBD86"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -147,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -164,10 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -464,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,116 +489,31 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>8</v>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction d'un oubli au niveau des reactions
</commit_message>
<xml_diff>
--- a/Config/Hmw_Tables/math.xlsx
+++ b/Config/Hmw_Tables/math.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Activité 112</t>
   </si>
@@ -43,10 +43,13 @@
     <t>Corrigé</t>
   </si>
   <si>
+    <t>Reçu</t>
+  </si>
+  <si>
+    <t>Skido</t>
+  </si>
+  <si>
     <t>Non rendu</t>
-  </si>
-  <si>
-    <t>Skido</t>
   </si>
 </sst>
 </file>
@@ -70,7 +73,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +107,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE8AE55"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBBD86"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -158,7 +167,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -503,17 +515,17 @@
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>9</v>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prise en compte des devoirs dans la range de deadline, début fix dans les cas ou il y a 2 hmw du même nom (pas dérangeant pour le merge
</commit_message>
<xml_diff>
--- a/Config/Hmw_Tables/math.xlsx
+++ b/Config/Hmw_Tables/math.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
-  <si>
-    <t>Activité 112</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Activité 23</t>
   </si>
@@ -34,16 +31,13 @@
     <t>Sloth</t>
   </si>
   <si>
-    <t>le 21/05 à 17:24</t>
-  </si>
-  <si>
-    <t>le 21/05 à 17:25</t>
-  </si>
-  <si>
-    <t>Corrigé</t>
-  </si>
-  <si>
     <t>Reçu</t>
+  </si>
+  <si>
+    <t>le 23/05 à 01:46</t>
+  </si>
+  <si>
+    <t>le 23/05 à 01:45</t>
   </si>
   <si>
     <t>Skido</t>
@@ -73,7 +67,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,19 +94,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFDFB3"/>
+        <fgColor rgb="FFEBBD86"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE8AE55"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBBD86"/>
+        <fgColor rgb="FFFFDFB3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -167,10 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -467,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,9 +462,9 @@
     <col min="2" max="702" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -490,42 +475,33 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>